<commit_message>
Simplified algo with a toggle register
</commit_message>
<xml_diff>
--- a/Algorithm/Instruction Set.xlsx
+++ b/Algorithm/Instruction Set.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="2" r:id="rId1"/>
     <sheet name="ISA" sheetId="3" r:id="rId2"/>
     <sheet name="u-ins" sheetId="4" r:id="rId3"/>
-    <sheet name="Sir eg" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sir eg" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="222">
   <si>
     <t>LDAC</t>
   </si>
@@ -119,9 +120,6 @@
     <t>MIDR</t>
   </si>
   <si>
-    <t>G0-G6</t>
-  </si>
-  <si>
     <t>No Operation</t>
   </si>
   <si>
@@ -150,9 +148,6 @@
   </si>
   <si>
     <t>AC &lt;- AC+R5</t>
-  </si>
-  <si>
-    <t>Inc AC by one</t>
   </si>
   <si>
     <t>Dec AC by one</t>
@@ -198,9 +193,6 @@
     <t>DIV4</t>
   </si>
   <si>
-    <t>K0-K3</t>
-  </si>
-  <si>
     <t>GENERAL</t>
   </si>
   <si>
@@ -273,13 +265,7 @@
     <t>0010 0010</t>
   </si>
   <si>
-    <t>0010 0011</t>
-  </si>
-  <si>
     <t>0100 0000</t>
-  </si>
-  <si>
-    <t>0100 0001</t>
   </si>
   <si>
     <t>0100 0010</t>
@@ -359,9 +345,6 @@
   </si>
   <si>
     <t>Data reg for d_mem</t>
-  </si>
-  <si>
-    <t>ISROW</t>
   </si>
   <si>
     <t>Kernel Registers</t>
@@ -395,9 +378,6 @@
 * 11 - write from bus</t>
   </si>
   <si>
-    <t>NUM</t>
-  </si>
-  <si>
     <t>CLR</t>
   </si>
   <si>
@@ -464,12 +444,6 @@
 return here</t>
   </si>
   <si>
-    <t>ATMP</t>
-  </si>
-  <si>
-    <t>Address Temp register</t>
-  </si>
-  <si>
     <t>ATMP &lt;- MIDR</t>
   </si>
   <si>
@@ -482,41 +456,9 @@
     <t>STOR</t>
   </si>
   <si>
-    <t>RCST</t>
-  </si>
-  <si>
-    <t>RCNG</t>
-  </si>
-  <si>
     <t>ZT</t>
   </si>
   <si>
-    <t>ZG</t>
-  </si>
-  <si>
-    <t>JPNZG</t>
-  </si>
-  <si>
-    <t>JPNZT</t>
-  </si>
-  <si>
-    <t>Manual flag
-1: if reading &amp; writing by row
-0: if reading &amp; writing by col</t>
-  </si>
-  <si>
-    <t>if (RCST = 0), means operation done</t>
-  </si>
-  <si>
-    <t>if (RCNG = 0), means array done</t>
-  </si>
-  <si>
-    <t>WCST</t>
-  </si>
-  <si>
-    <t>WCNG</t>
-  </si>
-  <si>
     <t>Constant half of address to be read</t>
   </si>
   <si>
@@ -553,21 +495,7 @@
     <t>Jump if z=0</t>
   </si>
   <si>
-    <t>Jump if ZT = 1
-(if RCST != 0)</t>
-  </si>
-  <si>
-    <t>Jump if ZG = 0
-(if RCNG != 0)</t>
-  </si>
-  <si>
     <t>JPNZ 62</t>
-  </si>
-  <si>
-    <t>JPNZT 62</t>
-  </si>
-  <si>
-    <t>JPNZG 62</t>
   </si>
   <si>
     <t>0010 0100</t>
@@ -638,6 +566,160 @@
   </si>
   <si>
     <t>?? How to close the control signals?</t>
+  </si>
+  <si>
+    <t>ZRT</t>
+  </si>
+  <si>
+    <t>ZRG</t>
+  </si>
+  <si>
+    <t>ZWT</t>
+  </si>
+  <si>
+    <t>ZWG</t>
+  </si>
+  <si>
+    <t>K0,K1</t>
+  </si>
+  <si>
+    <t>G0-G2</t>
+  </si>
+  <si>
+    <t>JNRT</t>
+  </si>
+  <si>
+    <t>JNRG</t>
+  </si>
+  <si>
+    <t>JNWT</t>
+  </si>
+  <si>
+    <t>JNWG</t>
+  </si>
+  <si>
+    <t>0010 0110</t>
+  </si>
+  <si>
+    <t>JNRG 62</t>
+  </si>
+  <si>
+    <t>JNWG 62</t>
+  </si>
+  <si>
+    <t>NEXT ADDRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JMPC</t>
+  </si>
+  <si>
+    <t>JUMPS</t>
+  </si>
+  <si>
+    <t>TOG</t>
+  </si>
+  <si>
+    <t>ZIR</t>
+  </si>
+  <si>
+    <t>ZIR   &lt;- !ZIR</t>
+  </si>
+  <si>
+    <t>TOG ZIR</t>
+  </si>
+  <si>
+    <t>A-BUS</t>
+  </si>
+  <si>
+    <t>I-BUS</t>
+  </si>
+  <si>
+    <t>Z-BUS</t>
+  </si>
+  <si>
+    <t>WRITE</t>
+  </si>
+  <si>
+    <t>READ-A</t>
+  </si>
+  <si>
+    <t>READ-I</t>
+  </si>
+  <si>
+    <t>READ-Z</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Manual flag, Togglable register
+1: Read along row: MDAR = A_T,A_G
+0: Read along col: MDAR = A_G,A_T</t>
+  </si>
+  <si>
+    <t>ZNRG</t>
+  </si>
+  <si>
+    <t>ZNWG</t>
+  </si>
+  <si>
+    <t>ZNRT</t>
+  </si>
+  <si>
+    <t>ZNWT</t>
+  </si>
+  <si>
+    <t>!(ARG = 0): still reading by row</t>
+  </si>
+  <si>
+    <t>!(AWG = 0): still writing by row</t>
+  </si>
+  <si>
+    <t>!(ART = 0): still reading by col</t>
+  </si>
+  <si>
+    <t>!(ART = 0): still writing by col</t>
+  </si>
+  <si>
+    <t>Jump if ZRG not 0
+(if ARG != 0)</t>
+  </si>
+  <si>
+    <t>Jump if ZWG not 0
+(if AWG != 0)</t>
+  </si>
+  <si>
+    <t>Jump if ZRT not 0
+(if ART != 0)</t>
+  </si>
+  <si>
+    <t>Jump if ZWG not 0
+(if AWT != 0)</t>
+  </si>
+  <si>
+    <t>Number of
+Registers</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>AWT</t>
+  </si>
+  <si>
+    <t>AWG</t>
+  </si>
+  <si>
+    <t>JNZT</t>
+  </si>
+  <si>
+    <t>Jump if tog not 1</t>
   </si>
 </sst>
 </file>
@@ -864,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -942,9 +1024,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -977,9 +1056,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1083,9 +1159,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1113,6 +1186,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1427,481 +1519,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="43" customWidth="1"/>
-    <col min="2" max="2" width="5" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13" style="42" customWidth="1"/>
-    <col min="4" max="6" width="5.5703125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="48.140625" style="44" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.42578125" style="41" customWidth="1"/>
+    <col min="2" max="2" width="13" style="40" customWidth="1"/>
+    <col min="3" max="5" width="5.5703125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="22.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49"/>
-      <c r="B1" s="27" t="s">
-        <v>119</v>
+    <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47"/>
+      <c r="B1" s="55" t="s">
+        <v>94</v>
       </c>
       <c r="C1" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="62">
+        <f>COUNTIF(B7:B23, "*")+1+2+1</f>
+        <v>17</v>
+      </c>
+      <c r="J1" s="91"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="48">
+        <v>8</v>
+      </c>
+      <c r="D2" s="48">
+        <v>1</v>
+      </c>
+      <c r="E2" s="48"/>
+      <c r="F2" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="77"/>
+      <c r="B3" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="49">
+        <v>8</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="77"/>
+      <c r="B4" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="49">
+        <v>8</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="77"/>
+      <c r="B5" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="49">
+        <v>8</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="59" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="78"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="C7" s="48">
+        <v>16</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48">
+        <v>2</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="50">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="77"/>
+      <c r="B8" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="49">
+        <v>8</v>
+      </c>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="77"/>
+      <c r="B9" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="49">
+        <v>8</v>
+      </c>
+      <c r="D9" s="49">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="50">
+      <c r="E9" s="49"/>
+      <c r="F9" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="77"/>
+      <c r="B10" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="49">
         <v>8</v>
       </c>
-      <c r="E2" s="50">
+      <c r="D10" s="49">
         <v>1</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="51">
-        <v>2</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="51">
+      <c r="E10" s="49"/>
+      <c r="F10" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="77"/>
+      <c r="B11" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="49">
         <v>8</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="40" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
-      <c r="B4" s="51">
-        <v>3</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="51">
+      <c r="D11" s="49">
+        <v>1</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="77"/>
+      <c r="B12" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="49">
         <v>8</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="51">
-        <v>4</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="51">
+      <c r="D12" s="49">
+        <v>1</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="78"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="45"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="48">
+        <v>1</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="A15" s="77"/>
+      <c r="B15" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="49">
+        <v>1</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="77"/>
+      <c r="B16" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="49">
+        <v>1</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="38" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="77"/>
+      <c r="B17" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="49">
+        <v>1</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="38" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="78"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="48">
+        <v>16</v>
+      </c>
+      <c r="D19" s="48">
+        <v>1</v>
+      </c>
+      <c r="E19" s="48"/>
+      <c r="F19" s="59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="77"/>
+      <c r="B20" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="49">
         <v>8</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="41" t="s">
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="60" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="51">
-        <v>5</v>
-      </c>
-      <c r="C6" s="55" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="51">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="77"/>
+      <c r="B21" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="49">
         <v>8</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="47"/>
-    </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="50">
-        <v>6</v>
-      </c>
-      <c r="C8" s="54" t="s">
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="50">
-        <v>16</v>
-      </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50">
-        <v>2</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="51">
-        <v>7</v>
-      </c>
-      <c r="C9" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="51">
-        <v>8</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="80"/>
-      <c r="B10" s="51">
-        <v>8</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="51">
-        <v>8</v>
-      </c>
-      <c r="E10" s="51">
-        <v>1</v>
-      </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="80"/>
-      <c r="B11" s="51">
-        <v>9</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="51">
-        <v>8</v>
-      </c>
-      <c r="E11" s="51">
-        <v>1</v>
-      </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="80"/>
-      <c r="B12" s="51">
-        <v>10</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="51">
-        <v>8</v>
-      </c>
-      <c r="E12" s="51">
-        <v>1</v>
-      </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="40" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="80"/>
-      <c r="B13" s="51">
-        <v>11</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="51">
-        <v>8</v>
-      </c>
-      <c r="E13" s="51">
-        <v>1</v>
-      </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="47"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="50">
-        <v>13</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="50">
-        <v>1</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-      <c r="B16" s="51">
-        <v>14</v>
-      </c>
-      <c r="C16" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="51">
-        <v>1</v>
-      </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="51">
-        <v>16</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="51">
-        <v>1</v>
-      </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="51">
-        <v>1</v>
-      </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="47"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="50">
-        <v>17</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="50">
-        <v>16</v>
-      </c>
-      <c r="E20" s="50">
-        <v>1</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="61" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="51">
-        <v>20</v>
-      </c>
-      <c r="C21" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="51">
-        <v>8</v>
-      </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="51">
-        <v>27</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="51">
-        <v>8</v>
-      </c>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="77"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="60"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="78"/>
       <c r="B23" s="51"/>
-      <c r="C23" s="55"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
       <c r="F23" s="51"/>
-      <c r="G23" s="62"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="81"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="60"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="C26" s="29"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="58"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="28"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="43"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="43"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="43"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="43"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
+      <c r="A35" s="43"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
+      <c r="A36" s="43"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
+      <c r="A37" s="43"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
+      <c r="A38" s="43"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
+      <c r="A39" s="43"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="43"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
+      <c r="A41" s="43"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="45"/>
+      <c r="A42" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A24"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1910,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1932,35 +1957,35 @@
     <row r="1" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" s="64">
-        <f>COUNTIF(B2:B32, "*")</f>
-        <v>25</v>
+        <v>62</v>
+      </c>
+      <c r="J1" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="62">
+        <f>COUNTIF(B2:B33, "*")</f>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
-        <v>56</v>
+      <c r="A2" s="79" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>1</v>
@@ -1969,17 +1994,17 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
+        <v>30</v>
+      </c>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="83"/>
+      <c r="A3" s="80"/>
       <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
@@ -1987,17 +2012,17 @@
         <v>0</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
+        <v>31</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="83"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="24" t="s">
         <v>24</v>
       </c>
@@ -2005,611 +2030,627 @@
         <v>0</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="32" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="83"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="34" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="80"/>
+      <c r="B6" s="24" t="s">
         <v>47</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="83"/>
-      <c r="B6" s="24" t="s">
-        <v>49</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="35" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="24" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="C7" s="12">
         <v>0</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>121</v>
-      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="23" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="80"/>
+      <c r="B8" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="81"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+    </row>
+    <row r="10" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="H9" s="77" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="G10" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="80"/>
+      <c r="B11" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="12">
         <v>1</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="12">
-        <v>0</v>
-      </c>
       <c r="D11" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
+        <v>144</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="80"/>
       <c r="B12" s="24" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="C12" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>19</v>
+        <v>147</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
+      <c r="A13" s="80"/>
       <c r="B13" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="12">
         <v>1</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="80"/>
+      <c r="B14" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H14" s="32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="84"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="81"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="24" t="s">
+      <c r="D16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="80"/>
+      <c r="B17" s="24" t="s">
         <v>6</v>
-      </c>
-      <c r="C16" s="12">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="33"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="24" t="s">
-        <v>7</v>
       </c>
       <c r="C17" s="12">
         <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="H17" s="33"/>
-    </row>
-    <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
+        <v>149</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="80"/>
       <c r="B18" s="24" t="s">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="C18" s="12">
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="H18" s="33"/>
-    </row>
-    <row r="19" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
+      <c r="F18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="80"/>
       <c r="B19" s="24" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>174</v>
-      </c>
+      <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="76" t="s">
-        <v>170</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="H19" s="33"/>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="38"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="82" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="23" t="s">
+      <c r="F19" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A20" s="80"/>
+      <c r="B20" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="80"/>
+      <c r="B21" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="81"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C23" s="9">
         <v>1</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11" t="s">
+      <c r="D23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="H23" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="12">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="80"/>
+      <c r="B24" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12">
         <v>0</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="33"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="12">
-        <v>1</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="33" t="s">
-        <v>22</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G24" s="31"/>
+      <c r="H24" s="32"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="33"/>
+        <v>41</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="38"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="23" t="s">
+      <c r="F26" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="80"/>
+      <c r="B27" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="81"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C29" s="9">
         <v>0</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="24" t="s">
+      <c r="D29" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="80"/>
+      <c r="B30" s="24" t="s">
         <v>12</v>
-      </c>
-      <c r="C29" s="12">
-        <v>0</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="24" t="s">
-        <v>13</v>
       </c>
       <c r="C30" s="12">
         <v>0</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="33"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
+      <c r="A31" s="80"/>
       <c r="B31" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="12">
         <v>0</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="33"/>
-    </row>
-    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="38"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" s="31"/>
+      <c r="H31" s="32"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="80"/>
+      <c r="B32" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="81"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>8</v>
-      </c>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
-      <c r="B41" s="28" t="s">
-        <v>92</v>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="85"/>
-      <c r="B42" s="2" t="s">
-        <v>93</v>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="82"/>
+      <c r="B42" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="82"/>
       <c r="B43" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
-      <c r="B44" s="28" t="s">
-        <v>27</v>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="82"/>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
-      <c r="B45" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="82"/>
+      <c r="B45" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="82"/>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="82"/>
+      <c r="B47" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2620,8 +2661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E175"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2630,1127 +2671,1127 @@
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.28515625" style="73" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" style="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65"/>
+      <c r="A1" s="63"/>
       <c r="B1" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="71" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="74" t="s">
-        <v>139</v>
+      <c r="E2" s="72" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="87"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="4" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
+      <c r="A4" s="84"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="75"/>
+        <v>123</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="73"/>
     </row>
     <row r="5" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
+      <c r="A5" s="84"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="75"/>
+        <v>125</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="73"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="87"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="75"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="73"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C7" s="24"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="75"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="73"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="75"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="73"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="87"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="24" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="E9" s="75"/>
+        <v>157</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="73"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="87"/>
+      <c r="A10" s="84"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>138</v>
+        <v>158</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="73" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="87"/>
+      <c r="A11" s="84"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="75"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="73"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="24" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" s="68" t="s">
-        <v>183</v>
-      </c>
-      <c r="E12" s="75" t="s">
-        <v>184</v>
+        <v>152</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="75"/>
+        <v>135</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="73"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
-        <v>57</v>
+      <c r="A14" s="84" t="s">
+        <v>54</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="75"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="73"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="24" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="D15" s="68" t="s">
-        <v>185</v>
-      </c>
-      <c r="E15" s="75" t="s">
-        <v>189</v>
+        <v>163</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="D16" s="68" t="s">
-        <v>188</v>
-      </c>
-      <c r="E16" s="75"/>
+        <v>164</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="73"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="75"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="73"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D18" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="75" t="s">
-        <v>190</v>
+        <v>169</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="73" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="87"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="68" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="75"/>
+        <v>170</v>
+      </c>
+      <c r="D19" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="73"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="87" t="s">
-        <v>58</v>
+      <c r="A20" s="84" t="s">
+        <v>55</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="75" t="s">
-        <v>195</v>
+        <v>171</v>
+      </c>
+      <c r="D20" s="66"/>
+      <c r="E20" s="73" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="75"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="73"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="75"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="73"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="87"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="75"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="73"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="87"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="75"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="73"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="87" t="s">
-        <v>59</v>
+      <c r="A25" s="84" t="s">
+        <v>56</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="75"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="73"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="87"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="75"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="73"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="87"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="75"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="73"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="73"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="75"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="73"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="75"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="73"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="75"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="73"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="87" t="s">
-        <v>60</v>
+      <c r="A32" s="84" t="s">
+        <v>57</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="75"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="73"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="87"/>
+      <c r="A33" s="84"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="75"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="73"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
+      <c r="A34" s="84"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="75"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="73"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="87"/>
+      <c r="A35" s="84"/>
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="75"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="73"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="87"/>
+      <c r="A36" s="84"/>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="73"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="75"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="73"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="75"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="73"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="75"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="73"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="86" t="s">
-        <v>96</v>
+      <c r="A40" s="83" t="s">
+        <v>91</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="75"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="73"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="86"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="75"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="73"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="86"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="75"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="73"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="86"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="75"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="73"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="86"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="75"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="73"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="86"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="75"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="73"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="86"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
-      <c r="D46" s="68"/>
-      <c r="E46" s="75"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="73"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="75"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="73"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="75"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="73"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="75"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="73"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="75"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="73"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="75"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="73"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="24"/>
       <c r="C52" s="24"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="75"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="73"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="24"/>
       <c r="C53" s="24"/>
-      <c r="D53" s="68"/>
-      <c r="E53" s="75"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="73"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="24"/>
       <c r="C54" s="24"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="75"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="73"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="24"/>
       <c r="C55" s="24"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="75"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="73"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="75"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="73"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="24"/>
       <c r="C57" s="24"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="75"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="73"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="75"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="73"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="75"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="73"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="24"/>
       <c r="C60" s="24"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="75"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="73"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="75"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="73"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="75"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="73"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="24"/>
       <c r="C63" s="24"/>
-      <c r="D63" s="68"/>
-      <c r="E63" s="75"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="73"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="24"/>
       <c r="C64" s="24"/>
-      <c r="D64" s="68"/>
-      <c r="E64" s="75"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="73"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="24"/>
       <c r="C65" s="24"/>
-      <c r="D65" s="68"/>
-      <c r="E65" s="75"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="73"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="75"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="73"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="24"/>
       <c r="C67" s="24"/>
-      <c r="D67" s="68"/>
-      <c r="E67" s="75"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="73"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="75"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="73"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
-      <c r="D69" s="68"/>
-      <c r="E69" s="75"/>
+      <c r="D69" s="66"/>
+      <c r="E69" s="73"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="75"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="73"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="75"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="73"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="24"/>
       <c r="C72" s="24"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="75"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="73"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="24"/>
       <c r="C73" s="24"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="75"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="73"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="24"/>
       <c r="C74" s="24"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="75"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="73"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
-      <c r="D75" s="68"/>
-      <c r="E75" s="75"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="73"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="75"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="73"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="75"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="73"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="75"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="73"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="75"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="73"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
-      <c r="D80" s="68"/>
-      <c r="E80" s="75"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="73"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="75"/>
+      <c r="D81" s="66"/>
+      <c r="E81" s="73"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="75"/>
+      <c r="D82" s="66"/>
+      <c r="E82" s="73"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="75"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="73"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="24"/>
       <c r="C84" s="24"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="75"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="73"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="24"/>
       <c r="C85" s="24"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="75"/>
+      <c r="D85" s="66"/>
+      <c r="E85" s="73"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="24"/>
       <c r="C86" s="24"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="75"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="73"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="24"/>
       <c r="C87" s="24"/>
-      <c r="D87" s="68"/>
-      <c r="E87" s="75"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="73"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="24"/>
       <c r="C88" s="24"/>
-      <c r="D88" s="68"/>
-      <c r="E88" s="75"/>
+      <c r="D88" s="66"/>
+      <c r="E88" s="73"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="24"/>
       <c r="C89" s="24"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="75"/>
+      <c r="D89" s="66"/>
+      <c r="E89" s="73"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="24"/>
       <c r="C90" s="24"/>
-      <c r="D90" s="68"/>
-      <c r="E90" s="75"/>
+      <c r="D90" s="66"/>
+      <c r="E90" s="73"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="24"/>
       <c r="C91" s="24"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="75"/>
+      <c r="D91" s="66"/>
+      <c r="E91" s="73"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
-      <c r="D92" s="68"/>
-      <c r="E92" s="75"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="73"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="24"/>
       <c r="C93" s="24"/>
-      <c r="D93" s="68"/>
-      <c r="E93" s="75"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="73"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="24"/>
       <c r="C94" s="24"/>
-      <c r="D94" s="68"/>
-      <c r="E94" s="75"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="73"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="24"/>
       <c r="C95" s="24"/>
-      <c r="D95" s="68"/>
-      <c r="E95" s="75"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="73"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="24"/>
       <c r="C96" s="24"/>
-      <c r="D96" s="68"/>
-      <c r="E96" s="75"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="73"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="24"/>
       <c r="C97" s="24"/>
-      <c r="D97" s="68"/>
-      <c r="E97" s="75"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="73"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="24"/>
       <c r="C98" s="24"/>
-      <c r="D98" s="68"/>
-      <c r="E98" s="75"/>
+      <c r="D98" s="66"/>
+      <c r="E98" s="73"/>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
-      <c r="D99" s="68"/>
-      <c r="E99" s="75"/>
+      <c r="D99" s="66"/>
+      <c r="E99" s="73"/>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="24"/>
       <c r="C100" s="24"/>
-      <c r="D100" s="68"/>
-      <c r="E100" s="75"/>
+      <c r="D100" s="66"/>
+      <c r="E100" s="73"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="24"/>
       <c r="C101" s="24"/>
-      <c r="D101" s="68"/>
+      <c r="D101" s="66"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="24"/>
       <c r="C102" s="24"/>
-      <c r="D102" s="68"/>
+      <c r="D102" s="66"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="24"/>
       <c r="C103" s="24"/>
-      <c r="D103" s="68"/>
+      <c r="D103" s="66"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
-      <c r="D104" s="68"/>
+      <c r="D104" s="66"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="24"/>
       <c r="C105" s="24"/>
-      <c r="D105" s="68"/>
+      <c r="D105" s="66"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="24"/>
       <c r="C106" s="24"/>
-      <c r="D106" s="68"/>
+      <c r="D106" s="66"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="24"/>
       <c r="C107" s="24"/>
-      <c r="D107" s="68"/>
+      <c r="D107" s="66"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="24"/>
       <c r="C108" s="24"/>
-      <c r="D108" s="68"/>
+      <c r="D108" s="66"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="24"/>
       <c r="C109" s="24"/>
-      <c r="D109" s="68"/>
+      <c r="D109" s="66"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="24"/>
       <c r="C110" s="24"/>
-      <c r="D110" s="68"/>
+      <c r="D110" s="66"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="24"/>
       <c r="C111" s="24"/>
-      <c r="D111" s="68"/>
+      <c r="D111" s="66"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="24"/>
       <c r="C112" s="24"/>
-      <c r="D112" s="68"/>
+      <c r="D112" s="66"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="24"/>
       <c r="C113" s="24"/>
-      <c r="D113" s="68"/>
+      <c r="D113" s="66"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="24"/>
       <c r="C114" s="24"/>
-      <c r="D114" s="68"/>
+      <c r="D114" s="66"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="24"/>
       <c r="C115" s="24"/>
-      <c r="D115" s="68"/>
+      <c r="D115" s="66"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
-      <c r="D116" s="68"/>
+      <c r="D116" s="66"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="24"/>
       <c r="C117" s="24"/>
-      <c r="D117" s="68"/>
+      <c r="D117" s="66"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="24"/>
       <c r="C118" s="24"/>
-      <c r="D118" s="68"/>
+      <c r="D118" s="66"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="24"/>
       <c r="C119" s="24"/>
-      <c r="D119" s="68"/>
+      <c r="D119" s="66"/>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="24"/>
       <c r="C120" s="24"/>
-      <c r="D120" s="68"/>
+      <c r="D120" s="66"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="24"/>
       <c r="C121" s="24"/>
-      <c r="D121" s="68"/>
+      <c r="D121" s="66"/>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="24"/>
       <c r="C122" s="24"/>
-      <c r="D122" s="68"/>
+      <c r="D122" s="66"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="24"/>
       <c r="C123" s="24"/>
-      <c r="D123" s="68"/>
+      <c r="D123" s="66"/>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="24"/>
       <c r="C124" s="24"/>
-      <c r="D124" s="68"/>
+      <c r="D124" s="66"/>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="24"/>
       <c r="C125" s="24"/>
-      <c r="D125" s="68"/>
+      <c r="D125" s="66"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="24"/>
       <c r="C126" s="24"/>
-      <c r="D126" s="68"/>
+      <c r="D126" s="66"/>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="24"/>
       <c r="C127" s="24"/>
-      <c r="D127" s="68"/>
+      <c r="D127" s="66"/>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="24"/>
       <c r="C128" s="24"/>
-      <c r="D128" s="68"/>
+      <c r="D128" s="66"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="24"/>
       <c r="C129" s="24"/>
-      <c r="D129" s="68"/>
+      <c r="D129" s="66"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="24"/>
       <c r="C130" s="24"/>
-      <c r="D130" s="68"/>
+      <c r="D130" s="66"/>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="24"/>
       <c r="C131" s="24"/>
-      <c r="D131" s="68"/>
+      <c r="D131" s="66"/>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="24"/>
       <c r="C132" s="24"/>
-      <c r="D132" s="68"/>
+      <c r="D132" s="66"/>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="24"/>
       <c r="C133" s="24"/>
-      <c r="D133" s="68"/>
+      <c r="D133" s="66"/>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="24"/>
       <c r="C134" s="24"/>
-      <c r="D134" s="68"/>
+      <c r="D134" s="66"/>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="24"/>
       <c r="C135" s="24"/>
-      <c r="D135" s="68"/>
+      <c r="D135" s="66"/>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="24"/>
       <c r="C136" s="24"/>
-      <c r="D136" s="68"/>
+      <c r="D136" s="66"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="24"/>
       <c r="C137" s="24"/>
-      <c r="D137" s="68"/>
+      <c r="D137" s="66"/>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="24"/>
       <c r="C138" s="24"/>
-      <c r="D138" s="68"/>
+      <c r="D138" s="66"/>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="24"/>
       <c r="C139" s="24"/>
-      <c r="D139" s="68"/>
+      <c r="D139" s="66"/>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="24"/>
       <c r="C140" s="24"/>
-      <c r="D140" s="68"/>
+      <c r="D140" s="66"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="24"/>
       <c r="C141" s="24"/>
-      <c r="D141" s="68"/>
+      <c r="D141" s="66"/>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="24"/>
       <c r="C142" s="24"/>
-      <c r="D142" s="68"/>
+      <c r="D142" s="66"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="24"/>
       <c r="C143" s="24"/>
-      <c r="D143" s="68"/>
+      <c r="D143" s="66"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="24"/>
       <c r="C144" s="24"/>
-      <c r="D144" s="68"/>
+      <c r="D144" s="66"/>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="24"/>
       <c r="C145" s="24"/>
-      <c r="D145" s="68"/>
+      <c r="D145" s="66"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="24"/>
       <c r="C146" s="24"/>
-      <c r="D146" s="68"/>
+      <c r="D146" s="66"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="24"/>
       <c r="C147" s="24"/>
-      <c r="D147" s="68"/>
+      <c r="D147" s="66"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="24"/>
       <c r="C148" s="24"/>
-      <c r="D148" s="68"/>
+      <c r="D148" s="66"/>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="24"/>
       <c r="C149" s="24"/>
-      <c r="D149" s="68"/>
+      <c r="D149" s="66"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="24"/>
       <c r="C150" s="24"/>
-      <c r="D150" s="68"/>
+      <c r="D150" s="66"/>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="24"/>
       <c r="C151" s="24"/>
-      <c r="D151" s="68"/>
+      <c r="D151" s="66"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="24"/>
       <c r="C152" s="24"/>
-      <c r="D152" s="68"/>
+      <c r="D152" s="66"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="24"/>
       <c r="C153" s="24"/>
-      <c r="D153" s="68"/>
+      <c r="D153" s="66"/>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="24"/>
       <c r="C154" s="24"/>
-      <c r="D154" s="68"/>
+      <c r="D154" s="66"/>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="24"/>
       <c r="C155" s="24"/>
-      <c r="D155" s="68"/>
+      <c r="D155" s="66"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="24"/>
       <c r="C156" s="24"/>
-      <c r="D156" s="68"/>
+      <c r="D156" s="66"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="24"/>
       <c r="C157" s="24"/>
-      <c r="D157" s="68"/>
+      <c r="D157" s="66"/>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="24"/>
       <c r="C158" s="24"/>
-      <c r="D158" s="68"/>
+      <c r="D158" s="66"/>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="24"/>
       <c r="C159" s="24"/>
-      <c r="D159" s="68"/>
+      <c r="D159" s="66"/>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="24"/>
       <c r="C160" s="24"/>
-      <c r="D160" s="68"/>
+      <c r="D160" s="66"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="24"/>
       <c r="C161" s="24"/>
-      <c r="D161" s="68"/>
+      <c r="D161" s="66"/>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="24"/>
       <c r="C162" s="24"/>
-      <c r="D162" s="68"/>
+      <c r="D162" s="66"/>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="24"/>
       <c r="C163" s="24"/>
-      <c r="D163" s="68"/>
+      <c r="D163" s="66"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="24"/>
       <c r="C164" s="24"/>
-      <c r="D164" s="68"/>
+      <c r="D164" s="66"/>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="24"/>
       <c r="C165" s="24"/>
-      <c r="D165" s="68"/>
+      <c r="D165" s="66"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="24"/>
       <c r="C166" s="24"/>
-      <c r="D166" s="68"/>
+      <c r="D166" s="66"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="24"/>
       <c r="C167" s="24"/>
-      <c r="D167" s="68"/>
+      <c r="D167" s="66"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="24"/>
       <c r="C168" s="24"/>
-      <c r="D168" s="68"/>
+      <c r="D168" s="66"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="24"/>
       <c r="C169" s="24"/>
-      <c r="D169" s="68"/>
+      <c r="D169" s="66"/>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="24"/>
       <c r="C170" s="24"/>
-      <c r="D170" s="68"/>
+      <c r="D170" s="66"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="24"/>
       <c r="C171" s="24"/>
-      <c r="D171" s="68"/>
+      <c r="D171" s="66"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="24"/>
       <c r="C172" s="24"/>
-      <c r="D172" s="68"/>
+      <c r="D172" s="66"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="24"/>
       <c r="C173" s="24"/>
-      <c r="D173" s="68"/>
+      <c r="D173" s="66"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="24"/>
       <c r="C174" s="24"/>
-      <c r="D174" s="68"/>
+      <c r="D174" s="66"/>
     </row>
     <row r="175" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B175" s="25"/>
       <c r="C175" s="25"/>
-      <c r="D175" s="70"/>
+      <c r="D175" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3768,10 +3809,300 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A16"/>
+  <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="85" customWidth="1"/>
+    <col min="2" max="57" width="3.7109375" style="85" customWidth="1"/>
+    <col min="58" max="16384" width="9.140625" style="85"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B1" s="85">
+        <v>0</v>
+      </c>
+      <c r="C1" s="85">
+        <v>1</v>
+      </c>
+      <c r="D1" s="85">
+        <v>2</v>
+      </c>
+      <c r="E1" s="85">
+        <v>3</v>
+      </c>
+      <c r="F1" s="85">
+        <v>4</v>
+      </c>
+      <c r="G1" s="85">
+        <v>5</v>
+      </c>
+      <c r="H1" s="85">
+        <v>6</v>
+      </c>
+      <c r="I1" s="85">
+        <v>7</v>
+      </c>
+      <c r="J1" s="85">
+        <v>8</v>
+      </c>
+      <c r="K1" s="85">
+        <v>9</v>
+      </c>
+      <c r="L1" s="85">
+        <v>10</v>
+      </c>
+      <c r="M1" s="85">
+        <v>11</v>
+      </c>
+      <c r="N1" s="85">
+        <v>12</v>
+      </c>
+      <c r="O1" s="85">
+        <v>13</v>
+      </c>
+      <c r="P1" s="85">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="85">
+        <v>15</v>
+      </c>
+      <c r="R1" s="85">
+        <v>16</v>
+      </c>
+      <c r="S1" s="85">
+        <v>17</v>
+      </c>
+      <c r="T1" s="85">
+        <v>18</v>
+      </c>
+      <c r="U1" s="85">
+        <v>19</v>
+      </c>
+      <c r="V1" s="85">
+        <v>20</v>
+      </c>
+      <c r="W1" s="85">
+        <v>21</v>
+      </c>
+      <c r="X1" s="85">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="85">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="85">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="85">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="85">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="85">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="85">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="85">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="85">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="85">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="85">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="85">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="85">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="85">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="85">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="85">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="85">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="85">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="85">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="85">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="85">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="85">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="85">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="85">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="85">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="86" t="s">
+        <v>188</v>
+      </c>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="88" t="s">
+        <v>192</v>
+      </c>
+      <c r="R2" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86"/>
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="86" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+      <c r="AQ2" s="86"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU2" s="86"/>
+      <c r="AV2" s="86"/>
+    </row>
+    <row r="3" spans="1:48" s="87" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" s="87" t="s">
+        <v>175</v>
+      </c>
+      <c r="P3" s="87" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="90"/>
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
+      <c r="AC3" s="90"/>
+      <c r="AD3" s="90"/>
+      <c r="AE3" s="90"/>
+      <c r="AF3" s="90"/>
+      <c r="AG3" s="90"/>
+      <c r="AH3" s="90"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AS2"/>
+    <mergeCell ref="AT2:AV2"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AH2"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:P2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3854,6 +4185,70 @@
         <v>14</v>
       </c>
     </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="49">
+        <v>1</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="38" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="49">
+        <v>1</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="38" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added some comments in ISA. trying to simulate the processor in Matlab
</commit_message>
<xml_diff>
--- a/Algorithm/Instruction Set.xlsx
+++ b/Algorithm/Instruction Set.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="230">
   <si>
     <t>LDAC</t>
   </si>
@@ -529,11 +529,6 @@
     <t>Jump if tog not 1</t>
   </si>
   <si>
-    <t>MDDR &lt;- M[a]
-* a = ARG, ART if(isRow = 1)
-* a = ART, ARG if(isRow = 0)</t>
-  </si>
-  <si>
     <t>MDAR &lt;- ART,ARG; Read</t>
   </si>
   <si>
@@ -576,12 +571,6 @@
     <t>OIN</t>
   </si>
   <si>
-    <t>OIA</t>
-  </si>
-  <si>
-    <t>OKA</t>
-  </si>
-  <si>
     <t>ORR</t>
   </si>
   <si>
@@ -591,12 +580,6 @@
     <t>Operand -&gt; if increment control signal</t>
   </si>
   <si>
-    <t>Operand -&gt; if jump ins address</t>
-  </si>
-  <si>
-    <t>Operand -&gt; if constant to be moved to AC</t>
-  </si>
-  <si>
     <t>Operand -&gt; if reg to be read</t>
   </si>
   <si>
@@ -607,11 +590,6 @@
   </si>
   <si>
     <t>RR</t>
-  </si>
-  <si>
-    <t>M[a] &lt;- AC
-* a = AWG, AWT if(isRow = 1)
-* a = AWT, AWG if(isRow = 0)</t>
   </si>
   <si>
     <t>JMPC</t>
@@ -751,6 +729,26 @@
 - K : Constant -&gt; A bus
 - RR: Reg name: R     -&gt; A bus
 - RW: Reg name: A bus -&gt; R</t>
+  </si>
+  <si>
+    <t>MDDR &lt;- M[a]
+* a = ARG, ART if(ZT = 0)
+* a = ART, ARG if(ZT = 1)</t>
+  </si>
+  <si>
+    <t>M[a] &lt;- AC
+* a = AWG, AWT if(ZT = 0)
+* a = AWT, AWG if(ZT = 1)</t>
+  </si>
+  <si>
+    <t>Iw
+Aw</t>
+  </si>
+  <si>
+    <t>CTRL</t>
+  </si>
+  <si>
+    <t>BINARY</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1206,6 +1204,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1215,6 +1289,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1237,89 +1320,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1706,7 @@
     <col min="2" max="2" width="13" style="36" customWidth="1"/>
     <col min="3" max="7" width="5.5703125" style="36" customWidth="1"/>
     <col min="8" max="8" width="48.140625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" style="104" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="87" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="18.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="4.140625" style="1" customWidth="1"/>
@@ -1701,33 +1714,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="62" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84"/>
-      <c r="B1" s="85" t="s">
+      <c r="A1" s="73"/>
+      <c r="B1" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="92" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" s="99" t="s">
-        <v>211</v>
+      <c r="E1" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="84" t="s">
+        <v>205</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="103" t="s">
-        <v>167</v>
+      <c r="I1" s="86" t="s">
+        <v>166</v>
       </c>
       <c r="K1" s="52" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="L1" s="53">
         <f>COUNTIF(B7:B25, "*")+1</f>
@@ -1735,7 +1748,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="99" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="47" t="s">
@@ -1748,21 +1761,21 @@
         <v>1</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>193</v>
-      </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="98"/>
+        <v>187</v>
+      </c>
+      <c r="F2" s="80"/>
+      <c r="G2" s="83"/>
       <c r="H2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="104" t="s">
-        <v>213</v>
+      <c r="I2" s="87" t="s">
+        <v>207</v>
       </c>
       <c r="K2" s="52"/>
       <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
+      <c r="A3" s="100"/>
       <c r="B3" s="48" t="s">
         <v>27</v>
       </c>
@@ -1771,21 +1784,21 @@
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="94"/>
+        <v>187</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="81"/>
       <c r="H3" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="104" t="s">
-        <v>213</v>
+      <c r="I3" s="87" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="48" t="s">
         <v>61</v>
       </c>
@@ -1794,19 +1807,19 @@
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
+        <v>187</v>
+      </c>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
       <c r="H4" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="104" t="s">
-        <v>213</v>
+      <c r="I4" s="87" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
+      <c r="A5" s="100"/>
       <c r="B5" s="48" t="s">
         <v>28</v>
       </c>
@@ -1814,39 +1827,39 @@
         <v>8</v>
       </c>
       <c r="D5" s="44"/>
-      <c r="E5" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="F5" s="94" t="s">
-        <v>194</v>
-      </c>
-      <c r="G5" s="94"/>
+      <c r="E5" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>227</v>
+      </c>
+      <c r="G5" s="81"/>
       <c r="H5" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="105" t="s">
-        <v>213</v>
+      <c r="I5" s="88" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="49"/>
       <c r="C6" s="45"/>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
       <c r="H6" s="41"/>
-      <c r="K6" s="100" t="s">
-        <v>206</v>
+      <c r="K6" s="85" t="s">
+        <v>200</v>
       </c>
       <c r="L6" s="4">
-        <f>COUNTIF(E$2:E$25, "Ir")</f>
+        <f>COUNTIF(E$2:E$25, "*Ir*")</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="99" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="47" t="s">
@@ -1857,28 +1870,28 @@
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43" t="s">
-        <v>175</v>
-      </c>
-      <c r="F7" s="93" t="s">
-        <v>195</v>
-      </c>
-      <c r="G7" s="93"/>
+        <v>174</v>
+      </c>
+      <c r="F7" s="80" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="80"/>
       <c r="H7" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="I7" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K7" s="100" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="88" t="s">
         <v>207</v>
       </c>
+      <c r="K7" s="85" t="s">
+        <v>201</v>
+      </c>
       <c r="L7" s="4">
-        <f>COUNTIF(F$2:F$25, "Iw")</f>
+        <f>COUNTIF(F$2:F$25, "*Iw*")</f>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="48" t="s">
         <v>69</v>
       </c>
@@ -1887,22 +1900,22 @@
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F8" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G8" s="94"/>
+        <v>190</v>
+      </c>
+      <c r="F8" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="81"/>
       <c r="H8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K8" s="100"/>
+      <c r="I8" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" s="85"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="48" t="s">
         <v>156</v>
       </c>
@@ -1913,30 +1926,30 @@
         <v>1</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G9" s="94" t="s">
-        <v>212</v>
+        <v>190</v>
+      </c>
+      <c r="F9" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="81" t="s">
+        <v>206</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K9" s="100" t="s">
-        <v>208</v>
+      <c r="I9" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="K9" s="85" t="s">
+        <v>202</v>
       </c>
       <c r="L9" s="4">
-        <f>COUNTIF(E$2:E$25, "Ar")</f>
+        <f>COUNTIF(E$2:E$25, "*Ar*")</f>
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
+      <c r="A10" s="100"/>
       <c r="B10" s="48" t="s">
         <v>157</v>
       </c>
@@ -1947,30 +1960,30 @@
         <v>1</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="94" t="s">
-        <v>212</v>
+        <v>190</v>
+      </c>
+      <c r="F10" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="81" t="s">
+        <v>206</v>
       </c>
       <c r="H10" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="I10" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K10" s="100" t="s">
-        <v>209</v>
+      <c r="I10" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="K10" s="85" t="s">
+        <v>203</v>
       </c>
       <c r="L10" s="4">
-        <f>COUNTIF(F$2:F$25, "Aw")</f>
-        <v>9</v>
+        <f>COUNTIF(F$2:F$25, "*Aw*")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
+      <c r="A11" s="100"/>
       <c r="B11" s="48" t="s">
         <v>158</v>
       </c>
@@ -1981,24 +1994,24 @@
         <v>1</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F11" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="94" t="s">
-        <v>212</v>
+        <v>190</v>
+      </c>
+      <c r="F11" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="G11" s="81" t="s">
+        <v>206</v>
       </c>
       <c r="H11" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K11" s="100"/>
+      <c r="I11" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="K11" s="85"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
+      <c r="A12" s="100"/>
       <c r="B12" s="48" t="s">
         <v>159</v>
       </c>
@@ -2009,41 +2022,41 @@
         <v>1</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F12" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G12" s="94" t="s">
-        <v>212</v>
+        <v>190</v>
+      </c>
+      <c r="F12" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="81" t="s">
+        <v>206</v>
       </c>
       <c r="H12" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="K12" s="101" t="s">
-        <v>210</v>
+      <c r="I12" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="K12" s="97" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="75"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="49"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
       <c r="H13" s="41"/>
-      <c r="K13" s="102"/>
+      <c r="K13" s="98"/>
       <c r="L13" s="4">
-        <f>COUNTIF(G$2:G$25, "x")</f>
+        <f>COUNTIF(G$2:G$25, "*x*")</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="99" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="47" t="s">
@@ -2054,21 +2067,21 @@
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>175</v>
-      </c>
-      <c r="G14" s="93"/>
+        <v>174</v>
+      </c>
+      <c r="G14" s="80"/>
       <c r="H14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="104" t="s">
-        <v>214</v>
+      <c r="I14" s="87" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="36" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
+      <c r="A15" s="100"/>
       <c r="B15" s="48" t="s">
         <v>98</v>
       </c>
@@ -2077,21 +2090,21 @@
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G15" s="94"/>
+        <v>174</v>
+      </c>
+      <c r="G15" s="81"/>
       <c r="H15" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="105" t="s">
-        <v>213</v>
+      <c r="I15" s="88" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
+      <c r="A16" s="100"/>
       <c r="B16" s="48" t="s">
         <v>144</v>
       </c>
@@ -2100,20 +2113,20 @@
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G16" s="94"/>
+        <v>174</v>
+      </c>
+      <c r="G16" s="81"/>
       <c r="H16" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="I16" s="105" t="s">
-        <v>213</v>
+      <c r="I16" s="88" t="s">
+        <v>207</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="L16" s="4">
         <f>COUNTIF(I$2:I$25, "D")</f>
@@ -2121,7 +2134,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
+      <c r="A17" s="100"/>
       <c r="B17" s="48" t="s">
         <v>146</v>
       </c>
@@ -2130,20 +2143,20 @@
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G17" s="94"/>
+        <v>174</v>
+      </c>
+      <c r="G17" s="81"/>
       <c r="H17" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="I17" s="105" t="s">
-        <v>213</v>
+      <c r="I17" s="88" t="s">
+        <v>207</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="L17" s="4">
         <f>COUNTIF(I$2:I$25, "G")+L16</f>
@@ -2151,17 +2164,17 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="75"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="49"/>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
       <c r="H18" s="41"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="99" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="47" t="s">
@@ -2174,126 +2187,126 @@
         <v>1</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H19" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="104" t="s">
-        <v>213</v>
+      <c r="I19" s="87" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
+      <c r="A20" s="100"/>
       <c r="B20" s="48" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C20" s="44">
         <v>8</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F20" s="44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="96" t="s">
-        <v>205</v>
-      </c>
-      <c r="I20" s="104" t="s">
-        <v>214</v>
+      <c r="H20" s="103" t="s">
+        <v>199</v>
+      </c>
+      <c r="I20" s="87" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="74"/>
+      <c r="A21" s="100"/>
       <c r="B21" s="48" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
       <c r="E21" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G21" s="44"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="104" t="s">
-        <v>214</v>
+      <c r="H21" s="103"/>
+      <c r="I21" s="87" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
+      <c r="A22" s="100"/>
       <c r="B22" s="48" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C22" s="44">
         <v>8</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G22" s="44"/>
-      <c r="H22" s="97" t="s">
-        <v>204</v>
-      </c>
-      <c r="I22" s="104" t="s">
-        <v>214</v>
+      <c r="H22" s="102" t="s">
+        <v>198</v>
+      </c>
+      <c r="I22" s="87" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
+      <c r="A23" s="100"/>
       <c r="B23" s="48" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="44"/>
       <c r="E23" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="G23" s="44"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="87" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="100"/>
+      <c r="B24" s="48" t="s">
         <v>196</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="104" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
-      <c r="B24" s="48" t="s">
-        <v>202</v>
       </c>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
       <c r="E24" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G24" s="44"/>
-      <c r="H24" s="96"/>
-      <c r="I24" s="104" t="s">
-        <v>214</v>
+      <c r="H24" s="103"/>
+      <c r="I24" s="87" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
+      <c r="A25" s="101"/>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -2301,7 +2314,7 @@
       <c r="F25" s="46"/>
       <c r="G25" s="46"/>
       <c r="H25" s="46"/>
-      <c r="I25" s="106"/>
+      <c r="I25" s="89"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H26" s="50"/>
@@ -2309,76 +2322,56 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
       <c r="B27" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="78">
+        <v>8</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="39"/>
+      <c r="B28" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="90">
+      <c r="C28" s="78">
         <v>8</v>
       </c>
-      <c r="E27" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="H27" s="38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="90">
-        <v>8</v>
-      </c>
       <c r="E28" s="36" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="39"/>
       <c r="B29" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="90">
+        <v>177</v>
+      </c>
+      <c r="C29" s="78">
         <v>8</v>
       </c>
       <c r="E29" s="36" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="39"/>
       <c r="B30" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="90">
-        <v>8</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="H30" s="38" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
-      <c r="B31" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="90">
-        <v>8</v>
-      </c>
-      <c r="E31" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="H31" s="38" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
@@ -2412,12 +2405,6 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="39"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2436,669 +2423,879 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="2"/>
-    <col min="3" max="3" width="5.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="1.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="41" style="3" customWidth="1"/>
-    <col min="8" max="8" width="4" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="3"/>
-    <col min="11" max="11" width="5.5703125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="17.28515625" style="3"/>
+    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="1.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="3"/>
+    <col min="12" max="12" width="5.5703125" style="3" customWidth="1"/>
+    <col min="13" max="14" width="17.28515625" style="3"/>
+    <col min="15" max="15" width="8.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="87" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="53">
+      <c r="L1" s="53">
         <f>COUNTIF(B2:B30, "*")</f>
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="105" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="110" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="114" t="str">
+        <f>DEC2BIN(O2)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="107"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="77"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="90"/>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="106"/>
       <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="115" t="str">
+        <f t="shared" ref="C3:C30" si="0">DEC2BIN(O3)</f>
+        <v>10</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="107" t="s">
-        <v>213</v>
-      </c>
-      <c r="J3" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="K3" s="4">
-        <f>COUNTIF(H$2:H$25, "D")</f>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3" s="4">
+        <f>COUNTIF(I$2:I$25, "D")</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
+      <c r="O3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="106"/>
       <c r="B4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
+      <c r="C4" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="G4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="H4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="107" t="s">
-        <v>214</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="K4" s="4">
-        <f>COUNTIF(H$2:H$25, "G")+K3</f>
+      <c r="I4" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="K4" s="64" t="s">
+        <v>223</v>
+      </c>
+      <c r="L4" s="4">
+        <f>COUNTIF(I$2:I$25, "G")+L3</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
+      <c r="O4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="106"/>
       <c r="B5" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30" t="s">
+      <c r="C5" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="108" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
+      <c r="I5" s="91" t="s">
+        <v>207</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="106"/>
       <c r="B6" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="C6" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="108" t="s">
-        <v>213</v>
-      </c>
-      <c r="J6" s="88" t="s">
-        <v>230</v>
-      </c>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="78"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="91" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6" s="104" t="s">
+        <v>224</v>
+      </c>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="107"/>
       <c r="B7" s="22"/>
-      <c r="C7" s="15"/>
+      <c r="C7" s="116" t="str">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
       <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="108"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-    </row>
-    <row r="8" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="91"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="105" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="110" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="D8" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="G8" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="H8" s="108" t="s">
-        <v>213</v>
-      </c>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
+      <c r="H8" s="66" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="91" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="106"/>
       <c r="B9" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="111" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="G9" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="H9" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="107"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-    </row>
-    <row r="10" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
+      <c r="I9" s="90"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="106"/>
       <c r="B10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="G10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="H10" s="108" t="s">
-        <v>213</v>
-      </c>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="77"/>
+      <c r="H10" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="91" t="s">
+        <v>207</v>
+      </c>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
+      <c r="O10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="106"/>
       <c r="B11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="111" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13" t="s">
+      <c r="C11" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="G11" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="H11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
+      <c r="I11" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="106"/>
       <c r="B12" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="111" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
+      <c r="C12" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="G12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="H12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="I12" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="107"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="107"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
+      <c r="C13" s="116" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="90"/>
+      <c r="O13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="105" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="110" t="s">
-        <v>173</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
+      <c r="C14" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+      <c r="D14" s="93" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="G14" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="107"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="90"/>
+      <c r="O14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="106"/>
       <c r="B15" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13" t="s">
+      <c r="C15" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="D15" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="G15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="107" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="O15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="106"/>
       <c r="B16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13" t="s">
+      <c r="C16" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="D16" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="G16" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="107"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="90"/>
+      <c r="O16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="106"/>
       <c r="B17" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13" t="s">
+      <c r="C17" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A18" s="106"/>
       <c r="B18" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="65" t="s">
+      <c r="C18" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10001</v>
+      </c>
+      <c r="D18" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="G18" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="106"/>
       <c r="B19" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="65" t="s">
+      <c r="C19" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10010</v>
+      </c>
+      <c r="D19" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="107"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="107"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="C20" s="116" t="str">
+        <f t="shared" si="0"/>
+        <v>10011</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="90"/>
+      <c r="O20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="110" t="s">
-        <v>187</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10" t="s">
+      <c r="C21" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>10100</v>
+      </c>
+      <c r="D21" s="93" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="G21" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="H21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
+      <c r="I21" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="100"/>
       <c r="B22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="111" t="s">
-        <v>174</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13" t="s">
+      <c r="C22" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10101</v>
+      </c>
+      <c r="D22" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="G22" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="H22" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
+      <c r="I22" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O22" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="100"/>
       <c r="B23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13" t="s">
+      <c r="C23" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10110</v>
+      </c>
+      <c r="D23" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="O23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="100"/>
       <c r="B24" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="111">
+      <c r="C24" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>10111</v>
+      </c>
+      <c r="D24" s="94">
         <v>1</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F24" s="27" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
+      <c r="H24" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="I24" s="27"/>
+      <c r="O24" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="101"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="18"/>
+      <c r="C25" s="116" t="str">
+        <f t="shared" si="0"/>
+        <v>11000</v>
+      </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="76" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="27"/>
+      <c r="O25" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="105" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="110" t="s">
-        <v>187</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
+      <c r="C26" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>11001</v>
+      </c>
+      <c r="D26" s="93" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="O26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="106"/>
       <c r="B27" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="111" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
+      <c r="C27" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>11010</v>
+      </c>
+      <c r="D27" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="27"/>
+      <c r="O27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="106"/>
       <c r="B28" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="111" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
+      <c r="C28" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>11011</v>
+      </c>
+      <c r="D28" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="27"/>
+      <c r="O28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="106"/>
       <c r="B29" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="111" t="s">
-        <v>187</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="78"/>
+      <c r="C29" s="115" t="str">
+        <f t="shared" si="0"/>
+        <v>11100</v>
+      </c>
+      <c r="D29" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="27"/>
+      <c r="O29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="107"/>
       <c r="B30" s="22"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="79" t="s">
+      <c r="C30" s="116" t="str">
+        <f t="shared" si="0"/>
+        <v>11101</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="27"/>
+      <c r="O30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="108" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="79"/>
-      <c r="B39" s="89" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="108"/>
+      <c r="B39" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="79"/>
+      <c r="C39" s="77"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="108"/>
       <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="79"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="108"/>
       <c r="B41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="79"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="108"/>
       <c r="B42" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="108"/>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="J6:M10"/>
+    <mergeCell ref="K6:N10"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="A38:A43"/>
     <mergeCell ref="A2:A7"/>
@@ -3106,7 +3303,7 @@
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"RR"</formula>
     </cfRule>
@@ -3164,7 +3361,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="110" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -3181,7 +3378,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
+      <c r="A3" s="110"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
         <v>85</v>
@@ -3194,7 +3391,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21" t="s">
         <v>86</v>
@@ -3205,7 +3402,7 @@
       <c r="E4" s="64"/>
     </row>
     <row r="5" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
+      <c r="A5" s="110"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21" t="s">
         <v>88</v>
@@ -3216,14 +3413,14 @@
       <c r="E5" s="64"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="57"/>
       <c r="E6" s="64"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="21" t="s">
         <v>93</v>
       </c>
@@ -3232,14 +3429,14 @@
       <c r="E7" s="64"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="57"/>
       <c r="E8" s="64"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="21" t="s">
         <v>103</v>
       </c>
@@ -3252,7 +3449,7 @@
       <c r="E9" s="64"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21" t="s">
         <v>115</v>
@@ -3265,14 +3462,14 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="57"/>
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="21" t="s">
         <v>96</v>
       </c>
@@ -3280,14 +3477,14 @@
         <v>111</v>
       </c>
       <c r="D12" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="E12" s="64" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="81"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>97</v>
@@ -3298,7 +3495,7 @@
       <c r="E13" s="64"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="110" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="21"/>
@@ -3307,35 +3504,35 @@
       <c r="E14" s="64"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="81"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="81"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>117</v>
@@ -3343,14 +3540,14 @@
       <c r="E17" s="64"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="57"/>
       <c r="E18" s="64"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="81"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="21" t="s">
         <v>3</v>
       </c>
@@ -3358,70 +3555,70 @@
         <v>119</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E19" s="64" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="57"/>
       <c r="E20" s="64"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="110" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E21" s="64"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="81"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="57"/>
       <c r="E22" s="64"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="81"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="57" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
+      <c r="A24" s="110"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="57"/>
       <c r="E24" s="64"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55"/>
       <c r="D25" s="57"/>
       <c r="E25" s="64"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="110" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="21"/>
@@ -3430,49 +3627,49 @@
       <c r="E26" s="64"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="57"/>
       <c r="E27" s="64"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="57"/>
       <c r="E28" s="64"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="81"/>
+      <c r="A29" s="110"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="57"/>
       <c r="E29" s="64"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="81"/>
+      <c r="A30" s="110"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="57"/>
       <c r="E30" s="64"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="81"/>
+      <c r="A31" s="110"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="57"/>
       <c r="E31" s="64"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="81"/>
+      <c r="A32" s="110"/>
       <c r="B32" s="55"/>
       <c r="C32" s="55"/>
       <c r="D32" s="57"/>
       <c r="E32" s="64"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="110" t="s">
         <v>47</v>
       </c>
       <c r="B33" s="21"/>
@@ -3481,28 +3678,28 @@
       <c r="E33" s="64"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
+      <c r="A34" s="110"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="57"/>
       <c r="E34" s="64"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="81"/>
+      <c r="A35" s="110"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
       <c r="D35" s="57"/>
       <c r="E35" s="64"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
+      <c r="A36" s="110"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
       <c r="D36" s="57"/>
       <c r="E36" s="64"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="81"/>
+      <c r="A37" s="110"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
       <c r="D37" s="57"/>
@@ -3530,7 +3727,7 @@
       <c r="E40" s="64"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="80" t="s">
+      <c r="A41" s="109" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="21"/>
@@ -3539,42 +3736,42 @@
       <c r="E41" s="64"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="80"/>
+      <c r="A42" s="109"/>
       <c r="B42" s="56"/>
       <c r="C42" s="56"/>
       <c r="D42" s="58"/>
       <c r="E42" s="64"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="80"/>
+      <c r="A43" s="109"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
       <c r="D43" s="57"/>
       <c r="E43" s="64"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="80"/>
+      <c r="A44" s="109"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
       <c r="D44" s="57"/>
       <c r="E44" s="64"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="80"/>
+      <c r="A45" s="109"/>
       <c r="B45" s="56"/>
       <c r="C45" s="56"/>
       <c r="D45" s="58"/>
       <c r="E45" s="64"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="80"/>
+      <c r="A46" s="109"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
       <c r="D46" s="57"/>
       <c r="E46" s="64"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="80"/>
+      <c r="A47" s="109"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="57"/>
@@ -4452,76 +4649,76 @@
       <c r="A2" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="82" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="91" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83" t="s">
-        <v>189</v>
-      </c>
-      <c r="N2" s="82" t="s">
+      <c r="B2" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="112" t="s">
+        <v>185</v>
+      </c>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" s="111" t="s">
         <v>132</v>
       </c>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="83" t="s">
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="113" t="s">
         <v>133</v>
       </c>
-      <c r="U2" s="82" t="s">
+      <c r="U2" s="111" t="s">
         <v>140</v>
       </c>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82"/>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82" t="s">
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111" t="s">
         <v>139</v>
       </c>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82"/>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82" t="s">
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="111" t="s">
         <v>138</v>
       </c>
-      <c r="AE2" s="82"/>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82" t="s">
+      <c r="AE2" s="111"/>
+      <c r="AF2" s="111"/>
+      <c r="AG2" s="111"/>
+      <c r="AH2" s="111"/>
+      <c r="AI2" s="111" t="s">
         <v>141</v>
       </c>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="82" t="s">
+      <c r="AJ2" s="111"/>
+      <c r="AK2" s="111"/>
+      <c r="AL2" s="111" t="s">
         <v>131</v>
       </c>
-      <c r="AM2" s="82"/>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82"/>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
+      <c r="AM2" s="111"/>
+      <c r="AN2" s="111"/>
+      <c r="AO2" s="111"/>
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="111"/>
+      <c r="AS2" s="111"/>
     </row>
     <row r="3" spans="1:45" s="68" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J3" s="72"/>
       <c r="K3" s="72"/>
       <c r="L3" s="72"/>
-      <c r="M3" s="83"/>
+      <c r="M3" s="113"/>
       <c r="N3" s="68" t="s">
         <v>15</v>
       </c>
@@ -4540,7 +4737,7 @@
       <c r="S3" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="T3" s="83"/>
+      <c r="T3" s="113"/>
       <c r="Y3" s="70" t="s">
         <v>75</v>
       </c>
@@ -4556,12 +4753,12 @@
       <c r="AC3" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="AD3" s="82" t="s">
+      <c r="AD3" s="111" t="s">
         <v>136</v>
       </c>
-      <c r="AE3" s="82"/>
-      <c r="AF3" s="82"/>
-      <c r="AG3" s="82"/>
+      <c r="AE3" s="111"/>
+      <c r="AF3" s="111"/>
+      <c r="AG3" s="111"/>
       <c r="AH3" s="69" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
ADR maker is updated
</commit_message>
<xml_diff>
--- a/Algorithm/Instruction Set.xlsx
+++ b/Algorithm/Instruction Set.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA\FPGA_shared\Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FED2FB90-807E-401F-BEB0-3D1EF84678CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{165C5E7A-3309-4CF2-B8AA-A1B3E72E2DC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="3" xr2:uid="{331EFD7D-ECF7-478D-B0E2-03D97775C47B}"/>
   </bookViews>
   <sheets>
@@ -680,19 +679,6 @@
     <t>G-Shift</t>
   </si>
   <si>
-    <t>0 -none
-1 -MDDR
-2 -ART
-3 -ARG
-4 -AWT
-5 -AWG
-6 -K0
-7 -K1
-8 -G
-11-MDIR
-15-all</t>
-  </si>
-  <si>
     <t>1-4</t>
   </si>
   <si>
@@ -1136,6 +1122,19 @@
   </si>
   <si>
     <t>11-14</t>
+  </si>
+  <si>
+    <t>0 -none
+1 -MDDR
+2 -ART
+3 -ARG
+4 -AWT
+5 -AWG
+6 -K0
+7 -K1
+8 -G
+9-MIDR
+15-all</t>
   </si>
 </sst>
 </file>
@@ -2606,10 +2605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2732,7 +2728,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
       <c r="B5" s="46" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" s="42">
         <v>6</v>
@@ -3353,10 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-    <sheetView topLeftCell="A8" workbookViewId="1">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -3513,7 +3506,7 @@
         <v>163</v>
       </c>
       <c r="J6" s="179" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K6" s="179"/>
       <c r="L6" s="179"/>
@@ -3523,17 +3516,17 @@
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="181"/>
       <c r="B7" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="164" t="s">
         <v>139</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="80"/>
@@ -3590,17 +3583,17 @@
     <row r="10" spans="1:14" ht="54" x14ac:dyDescent="0.25">
       <c r="A10" s="181"/>
       <c r="B10" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C10" s="150" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>275</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>276</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="80"/>
@@ -4125,11 +4118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-    <sheetView topLeftCell="A25" workbookViewId="1">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4153,7 +4143,7 @@
         <v>79</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>87</v>
@@ -4171,13 +4161,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E3" s="170"/>
       <c r="F3" s="11"/>
@@ -4196,10 +4186,10 @@
         <v>84</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4214,7 +4204,7 @@
         <v>102</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" s="57"/>
     </row>
@@ -4230,7 +4220,7 @@
         <v>86</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F6" s="57" t="s">
         <v>88</v>
@@ -4245,10 +4235,10 @@
         <v>85</v>
       </c>
       <c r="D7" s="54" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="58" t="s">
         <v>306</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>307</v>
       </c>
       <c r="F7" s="57"/>
     </row>
@@ -4256,10 +4246,10 @@
       <c r="A8" s="168"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" s="54" t="s">
         <v>308</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>309</v>
       </c>
       <c r="E8" s="58"/>
       <c r="F8" s="57"/>
@@ -4296,7 +4286,7 @@
         <v>102</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="57"/>
     </row>
@@ -4309,10 +4299,10 @@
         <v>105</v>
       </c>
       <c r="D11" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="F11" s="57"/>
     </row>
@@ -4322,13 +4312,13 @@
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D12" s="54" t="s">
         <v>193</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" s="57" t="s">
         <v>89</v>
@@ -4339,16 +4329,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="D13" s="54" t="s">
         <v>201</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F13" s="57"/>
     </row>
@@ -4358,13 +4348,13 @@
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F14" s="57"/>
     </row>
@@ -4374,13 +4364,13 @@
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F15" s="57"/>
     </row>
@@ -4390,13 +4380,13 @@
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" s="54" t="s">
         <v>201</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F16" s="57"/>
     </row>
@@ -4406,13 +4396,13 @@
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F17" s="57"/>
     </row>
@@ -4422,13 +4412,13 @@
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F18" s="57"/>
     </row>
@@ -4438,13 +4428,13 @@
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" s="54" t="s">
         <v>102</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F19" s="57"/>
     </row>
@@ -4454,13 +4444,13 @@
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D20" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="F20" s="57"/>
     </row>
@@ -4470,13 +4460,13 @@
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F21" s="57"/>
     </row>
@@ -4486,13 +4476,13 @@
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F22" s="57"/>
     </row>
@@ -4502,13 +4492,13 @@
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="D23" s="54" t="s">
-        <v>258</v>
-      </c>
       <c r="E23" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F23" s="57"/>
     </row>
@@ -4523,10 +4513,10 @@
         <v>101</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F24" s="57" t="s">
         <v>128</v>
@@ -4544,7 +4534,7 @@
         <v>102</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F25" s="57"/>
     </row>
@@ -4554,13 +4544,13 @@
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" s="54" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="57"/>
     </row>
@@ -4575,10 +4565,10 @@
         <v>168</v>
       </c>
       <c r="D27" s="54" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.25">
@@ -4593,7 +4583,7 @@
         <v>194</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F28" s="57" t="s">
         <v>129</v>
@@ -4613,7 +4603,7 @@
         <v>102</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F29" s="57"/>
     </row>
@@ -4629,7 +4619,7 @@
         <v>198</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F30" s="57" t="s">
         <v>106</v>
@@ -4649,7 +4639,7 @@
         <v>102</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F31" s="57"/>
     </row>
@@ -4665,7 +4655,7 @@
         <v>199</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F32" s="57"/>
     </row>
@@ -4677,13 +4667,13 @@
         <v>4</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D33" s="54" t="s">
         <v>201</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F33" s="57"/>
     </row>
@@ -4693,13 +4683,13 @@
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>287</v>
+      </c>
+      <c r="E34" s="58" t="s">
         <v>286</v>
-      </c>
-      <c r="D34" s="54" t="s">
-        <v>288</v>
-      </c>
-      <c r="E34" s="58" t="s">
-        <v>287</v>
       </c>
       <c r="F34" s="56"/>
     </row>
@@ -4711,13 +4701,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D35" s="54" t="s">
         <v>201</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F35" s="56"/>
     </row>
@@ -4727,13 +4717,13 @@
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D36" s="54" t="s">
+        <v>288</v>
+      </c>
+      <c r="E36" s="58" t="s">
         <v>289</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>290</v>
       </c>
       <c r="F36" s="56"/>
     </row>
@@ -4751,7 +4741,7 @@
         <v>201</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F37" s="56"/>
     </row>
@@ -4767,7 +4757,7 @@
         <v>200</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F38" s="57"/>
     </row>
@@ -4785,7 +4775,7 @@
         <v>102</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F39" s="57"/>
     </row>
@@ -4798,10 +4788,10 @@
         <v>189</v>
       </c>
       <c r="D40" s="54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F40" s="57"/>
     </row>
@@ -4813,13 +4803,13 @@
         <v>53</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D41" s="52" t="s">
         <v>102</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F41" s="57"/>
     </row>
@@ -4829,13 +4819,13 @@
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D42" s="54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E42" s="58" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F42" s="57"/>
     </row>
@@ -4850,10 +4840,10 @@
         <v>21</v>
       </c>
       <c r="D43" s="54" t="s">
+        <v>279</v>
+      </c>
+      <c r="E43" s="58" t="s">
         <v>280</v>
-      </c>
-      <c r="E43" s="58" t="s">
-        <v>281</v>
       </c>
       <c r="F43" s="57"/>
     </row>
@@ -4871,7 +4861,7 @@
         <v>195</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F44" s="57"/>
     </row>
@@ -4886,10 +4876,10 @@
         <v>191</v>
       </c>
       <c r="D45" s="54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F45" s="57"/>
     </row>
@@ -4907,7 +4897,7 @@
         <v>196</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F46" s="57"/>
     </row>
@@ -4925,7 +4915,7 @@
         <v>197</v>
       </c>
       <c r="E47" s="58" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F47" s="88"/>
     </row>
@@ -5782,10 +5772,7 @@
   <dimension ref="A1:AH55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:AC3"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,43 +5802,43 @@
         <v>0</v>
       </c>
       <c r="C1" s="122" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="E1" s="124" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="124" t="s">
-        <v>209</v>
-      </c>
       <c r="F1" s="125" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G1" s="126" t="s">
+        <v>225</v>
+      </c>
+      <c r="H1" s="126" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="126" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="122" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="126" t="s">
-        <v>219</v>
-      </c>
-      <c r="I1" s="126" t="s">
-        <v>220</v>
-      </c>
-      <c r="J1" s="122" t="s">
-        <v>227</v>
-      </c>
       <c r="K1" s="119" t="s">
+        <v>216</v>
+      </c>
+      <c r="L1" s="144" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="144" t="s">
-        <v>218</v>
-      </c>
       <c r="M1" s="152" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N1" s="157" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O1" s="127" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5862,19 +5849,19 @@
         <v>111</v>
       </c>
       <c r="C2" s="137" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="138" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="139" t="s">
         <v>223</v>
-      </c>
-      <c r="D2" s="138" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" s="139" t="s">
-        <v>224</v>
       </c>
       <c r="F2" s="140" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="184" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H2" s="184"/>
       <c r="I2" s="184"/>
@@ -5882,19 +5869,19 @@
         <v>113</v>
       </c>
       <c r="K2" s="143" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L2" s="145" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M2" s="153" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N2" s="158" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O2" s="141" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="60" customFormat="1" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5903,19 +5890,19 @@
         <v>204</v>
       </c>
       <c r="C3" s="130" t="s">
-        <v>206</v>
+        <v>311</v>
       </c>
       <c r="D3" s="131" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" s="132" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F3" s="133" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G3" s="134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H3" s="134" t="s">
         <v>203</v>
@@ -5924,23 +5911,23 @@
         <v>202</v>
       </c>
       <c r="J3" s="130" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K3" s="148" t="s">
         <v>205</v>
       </c>
       <c r="L3" s="149" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M3" s="154" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N3" s="159" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O3" s="135"/>
       <c r="U3" s="185" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="V3" s="185"/>
       <c r="W3" s="185"/>

</xml_diff>